<commit_message>
Added formula handling functionality Added cells merging option Some test file clarifications
</commit_message>
<xml_diff>
--- a/examples/books-output.xlsx
+++ b/examples/books-output.xlsx
@@ -13,7 +13,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <si>
-    <t>{{ | | library }}</t>
+    <t>{{ | | library.name }}</t>
   </si>
   <si>
     <t>Criteria \ Books</t>
@@ -1696,7 +1696,7 @@
     <col min="29" max="29" width="25.1719" style="1" customWidth="1"/>
     <col min="30" max="30" width="16.3516" style="1" customWidth="1"/>
     <col min="31" max="31" width="25.1719" style="1" customWidth="1"/>
-    <col min="32" max="256" width="16.3516" style="1" customWidth="1"/>
+    <col min="32" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">

</xml_diff>